<commit_message>
fix image urls (#4)
</commit_message>
<xml_diff>
--- a/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
+++ b/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMD\Documents\UiPath\Is prof extractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E155C440-9729-4A4C-855E-AE02395CFE7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462EA7EF-9818-4DEC-9E45-782FDFC61839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="257">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -371,9 +371,6 @@
     <t>CHENARU Oana Gabriela</t>
   </si>
   <si>
-    <t>Dobrescu Radu Nicolae</t>
-  </si>
-  <si>
     <t>DOBRICA Liliana</t>
   </si>
   <si>
@@ -383,12 +380,6 @@
     <t>FAGARASAN Ioana</t>
   </si>
   <si>
-    <t>Hossu Andrei</t>
-  </si>
-  <si>
-    <t>Hossu Daniela</t>
-  </si>
-  <si>
     <t>IACOB Iulia-Lidia</t>
   </si>
   <si>
@@ -404,9 +395,6 @@
     <t>MEREZEANU Daniel Marian</t>
   </si>
   <si>
-    <t>Mocanu Stefan Alexandru</t>
-  </si>
-  <si>
     <t>MOISESCU Mihnea Alexandru</t>
   </si>
   <si>
@@ -440,9 +428,6 @@
     <t>STAMATESCU Grigore</t>
   </si>
   <si>
-    <t>Stamatescu Iulia</t>
-  </si>
-  <si>
     <t>VLAD Madalin</t>
   </si>
   <si>
@@ -476,9 +461,6 @@
     <t>/index.php?option=com_content&amp;view=article&amp;id=851:cv-chenaru-oana&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
-    <t>/index.php?option=com_content&amp;view=article&amp;id=55:cv-dobrescu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>/index.php?option=com_content&amp;view=article&amp;id=824:cv-dobrica-liliana&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
@@ -488,12 +470,6 @@
     <t>/index.php?option=com_content&amp;view=article&amp;id=825:cv-fagarasan-ioana&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
-    <t>/index.php?option=com_content&amp;view=article&amp;id=27:cv-hossuandrei&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>/index.php?option=com_content&amp;view=article&amp;id=36:cv-hossu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>/index.php?option=com_content&amp;view=article&amp;id=853:cv-iacob-iulia&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
@@ -509,9 +485,6 @@
     <t>/index.php?option=com_content&amp;view=article&amp;id=833:cv-merezeanu-daniel&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
-    <t>/index.php?option=com_content&amp;view=article&amp;id=63:cv-mocanu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>/index.php?option=com_content&amp;view=article&amp;id=852:cv-moisescu-mihnea&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
@@ -545,9 +518,6 @@
     <t>/index.php?option=com_content&amp;view=article&amp;id=826:cv-stamatescu-grigore&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
-    <t>/index.php?option=com_content&amp;view=article&amp;id=227:cv-stamatescu-iulia&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>/index.php?option=com_content&amp;view=article&amp;id=843:cv-vlad-madalin&amp;catid=7:upb&amp;Itemid=11</t>
   </si>
   <si>
@@ -575,9 +545,6 @@
     <t>Sef lucrari dr.ing.</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=841:cv-anghel-magdalena&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED309</t>
   </si>
   <si>
@@ -587,277 +554,298 @@
     <t>Conferentiar dr.ing.</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=832:cv-anton-florin&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED111</t>
   </si>
   <si>
     <t>silvia.anton@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=859:cv-anton-silvia&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED212/PR406</t>
   </si>
   <si>
     <t>nicoleta.arghira@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=858:cv-arghira-nicoleta&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>theodor.borangiu@upb.ro</t>
   </si>
   <si>
     <t>Profesor dr.ing., coordonator doctorat</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=845:cv-borangiu-theodor&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED115</t>
   </si>
   <si>
     <t>vasile.calofir@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=854:cv-calofir-vasile&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED209</t>
   </si>
   <si>
     <t>simona.caramihai@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=848:cv-caramihai-simona&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED415</t>
   </si>
   <si>
     <t>alexandra.cernian@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=834:cv-cernian-alexandra&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED303</t>
   </si>
   <si>
     <t>oana.chenaru@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=851:cv-chenaru-oana&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>rd_dobrescu@yahoo.com</t>
-  </si>
-  <si>
-    <t>021/402.91.05</t>
-  </si>
-  <si>
     <t>liliana.dobrica@upb.ro</t>
   </si>
   <si>
     <t>Profesor dr.ing.</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=824%3Acv-dobrica-liliana&amp;catid=7%3Aupb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED413</t>
   </si>
   <si>
     <t>alexandru.dumitrache@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=860:cv-dumitrache-alexandru&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED212/ PRECIS 406</t>
   </si>
   <si>
     <t>ioana.fagarasan@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=825:cv-fagarasan-ioana&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>dana@aii.pub.ro</t>
-  </si>
-  <si>
     <t>iulia.iacob@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=853:cv-iacob-iulia&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED305/ PRECIS 403</t>
   </si>
   <si>
     <t>loretta.ichim@upb.ro</t>
   </si>
   <si>
-    <t>Conferentiar dr.ing., coordonator doctorat</t>
-  </si>
-  <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=831:cv-ichim-loretta&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED415, PRECIS 401</t>
   </si>
   <si>
     <t>anca.ionita@upb.ro</t>
   </si>
   <si>
-    <t>Profesor dr.ing., conducator doctorat</t>
-  </si>
-  <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=835:cv-ionita-anca&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>nik.ivanescu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=846:cv-ivanescu-nik-andrei&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED305</t>
   </si>
   <si>
     <t>daniel.merezeanu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=833:cv-merezeanu-daniel&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>smocanu@rdslink.ro</t>
-  </si>
-  <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=63:cv-mocanu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED209-210</t>
   </si>
   <si>
     <t>mihnea.moisescu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=852:cv-moisescu-mihnea&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED211-212</t>
   </si>
   <si>
     <t>cristina.nichiforov@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=850:cv-nichiforov-cristina&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>max.nicolae@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=827:cv-nicolae-maximilian&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ecaterina.oltean@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=855:cv-oltean-cati&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>adriana.olteanu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=836:cv-olteanu-adriana&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>radu.pietraru@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=828:cv-pietraru-radu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED305, PRECIS 403</t>
   </si>
   <si>
     <t>dan.popescu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=830:cv-popescu-dan&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>silviu.raileanu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=842:cv-raileanu-silviu&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED406</t>
   </si>
   <si>
     <t>daniela.saru@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=856:cv-saru-daniela&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>ED212</t>
   </si>
   <si>
     <t>mircea_stefan.simoiu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=849:cv-simoiu-mircea&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
     <t>PRECIS 406</t>
   </si>
   <si>
     <t>grigore.stamatescu@upb.ro</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=826:cv-stamatescu-grigore&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>iulia.stamatescu@aii.pub.ro</t>
-  </si>
-  <si>
-    <t>021/402.91.47</t>
-  </si>
-  <si>
     <t>madalin.vlad@upb.ro</t>
   </si>
   <si>
     <t>SL dr.ing.</t>
   </si>
   <si>
-    <t>http://www.aii.pub.ro/index.php?option=com_content&amp;view=article&amp;id=843:cv-vlad-madalin&amp;catid=7:upb&amp;Itemid=11</t>
-  </si>
-  <si>
-    <t>Conf.dr. Ing.</t>
-  </si>
-  <si>
     <t>As. drd.ing.</t>
   </si>
   <si>
     <t>As. dr.ing.</t>
   </si>
   <si>
-    <t>Conf.dr.ing.</t>
-  </si>
-  <si>
-    <t>Prof.dr.ing.</t>
-  </si>
-  <si>
-    <t>Prof.dr.ing</t>
-  </si>
-  <si>
-    <t>Prof. dr. ing., conducator doctorat din anul 1991 in domeniul Automatica (in prezent Ingineria Sistemelor)</t>
+    <t>/images/Poze_cadre_didactice/anghel_magda.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/anton_florin.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/anton_silvia.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/arghira_nicoleta.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/borangiu_theodor.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/calofir_vasile.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/caramihai_simona.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/cernian_alexandra.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/chenaru_oana.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/dobrica_liliana.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/dumitrache_alexandru.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/fagarasan_ioana.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/iacob_lidia.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/ichim_loretta.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/ionita_anca_2.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/ivanescu_nick.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/merezeanu_daniel.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/moisescu_mihnea.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/nichiforov_cristina.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/nicolae_maximilian.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/zzz.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/olteanu_adriana.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/pietraru_radu.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/popescu_dan.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/raileanu_silviu.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/saru_daniela.jpg</t>
+  </si>
+  <si>
+    <t>DOBRESCU Radu</t>
+  </si>
+  <si>
+    <t>/index.php?option=com_content&amp;view=article&amp;id=868:cv-dobrescu-radu&amp;catid=7:upb&amp;Itemid=11</t>
+  </si>
+  <si>
+    <t>HOSSU Andrei</t>
+  </si>
+  <si>
+    <t>/index.php?option=com_content&amp;view=article&amp;id=866:cv-hossu-andrei&amp;catid=7:upb&amp;Itemid=11</t>
+  </si>
+  <si>
+    <t>HOSSU Daniela</t>
+  </si>
+  <si>
+    <t>/index.php?option=com_content&amp;view=article&amp;id=865:cv-hossu-daniela&amp;catid=7:upb&amp;Itemid=11</t>
+  </si>
+  <si>
+    <t>MOCANU Stefan Alexandru</t>
+  </si>
+  <si>
+    <t>/index.php?option=com_content&amp;view=article&amp;id=870:cv-mocanu-stefan&amp;catid=7:upb&amp;Itemid=11</t>
+  </si>
+  <si>
+    <t>STAMATESCU Iulia Vasilica</t>
+  </si>
+  <si>
+    <t>/index.php?option=com_content&amp;view=article&amp;id=867:cv-stamatescu-iuia&amp;catid=7:upb&amp;Itemid=11</t>
+  </si>
+  <si>
+    <t>Educatie</t>
+  </si>
+  <si>
+    <t>radu.dobrescu@upb.ro</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/radu_dobrescu.jpg</t>
+  </si>
+  <si>
+    <t>ED414</t>
+  </si>
+  <si>
+    <t>andrei.hossu@upb.ro</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/andrei_hossu.jpg</t>
+  </si>
+  <si>
+    <t>daniela.hossu@upb.ro</t>
+  </si>
+  <si>
+    <t>stefan.mocanu@upb.ro</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/st_moc.jpg</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/stamatescu_grigore.jpg</t>
+  </si>
+  <si>
+    <t>ED213/ PRECIS 406</t>
+  </si>
+  <si>
+    <t>iulia.stamatescu@upb.ro</t>
+  </si>
+  <si>
+    <t>/images/Poze_cadre_didactice/iulia_stamatescu.jpg</t>
   </si>
 </sst>
 </file>
@@ -872,7 +860,7 @@
     <numFmt numFmtId="165" formatCode="yyyy;@"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -990,12 +978,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1329,7 +1311,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1414,10 +1396,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2026,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C8" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2037,7 +2015,7 @@
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="48.28515625" customWidth="1"/>
     <col min="7" max="7" width="37.42578125" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
@@ -2047,22 +2025,22 @@
         <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F1" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2070,19 +2048,19 @@
         <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2090,19 +2068,19 @@
         <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
       <c r="G3" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2110,19 +2088,19 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2130,19 +2108,19 @@
         <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="E5" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="F5" t="s">
-        <v>176</v>
+        <v>211</v>
       </c>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2150,19 +2128,19 @@
         <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="G6" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2170,19 +2148,19 @@
         <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
-      </c>
-      <c r="G7" s="42" t="s">
-        <v>252</v>
+        <v>213</v>
+      </c>
+      <c r="G7" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2190,19 +2168,19 @@
         <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>195</v>
+        <v>214</v>
+      </c>
+      <c r="G8" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2210,19 +2188,19 @@
         <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="E9" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="G9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2230,498 +2208,516 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="E10" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
-      </c>
-      <c r="G10" s="42" t="s">
-        <v>165</v>
+        <v>216</v>
+      </c>
+      <c r="G10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
-        <v>133</v>
+        <v>235</v>
       </c>
       <c r="C11" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G11" s="48" t="s">
-        <v>260</v>
+        <v>245</v>
+      </c>
+      <c r="E11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" t="s">
+        <v>246</v>
+      </c>
+      <c r="G11" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="E12" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F12" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C13" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="E13" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
       <c r="G13" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="F14" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="G14" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>259</v>
+        <v>237</v>
+      </c>
+      <c r="C15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" t="s">
+        <v>247</v>
+      </c>
+      <c r="F15" t="s">
+        <v>249</v>
+      </c>
+      <c r="G15" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
-        <v>138</v>
+        <v>239</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" t="s">
-        <v>193</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>258</v>
+        <v>250</v>
+      </c>
+      <c r="E16" t="s">
+        <v>171</v>
+      </c>
+      <c r="F16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G16" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="E17" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F17" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
       <c r="G17" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="E18" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="F18" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="F19" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="G19" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
-        <v>215</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>169</v>
+        <v>223</v>
+      </c>
+      <c r="G20" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="F21" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="G21" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>109</v>
+        <v>240</v>
       </c>
       <c r="B22" t="s">
-        <v>144</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
-        <v>219</v>
-      </c>
-      <c r="D22" t="s">
-        <v>193</v>
+        <v>251</v>
+      </c>
+      <c r="E22" t="s">
+        <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>220</v>
-      </c>
-      <c r="G22" s="42" t="s">
-        <v>257</v>
+        <v>252</v>
+      </c>
+      <c r="G22" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="E23" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="F23" t="s">
-        <v>223</v>
-      </c>
-      <c r="G23" s="48" t="s">
-        <v>178</v>
+        <v>225</v>
+      </c>
+      <c r="G23" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="E24" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="F24" t="s">
         <v>226</v>
       </c>
-      <c r="G24" s="42" t="s">
-        <v>256</v>
+      <c r="G24" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" t="s">
         <v>227</v>
       </c>
-      <c r="E25" t="s">
-        <v>189</v>
-      </c>
-      <c r="F25" t="s">
-        <v>228</v>
-      </c>
       <c r="G25" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B26" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C26" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="E26" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F26" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G26" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="E27" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="F27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="G27" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B28" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="E28" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="F28" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G28" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="E29" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="F29" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="G29" t="s">
-        <v>178</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>238</v>
+        <v>197</v>
       </c>
       <c r="E30" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F30" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="G30" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="E31" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="F31" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="G31" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C32" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
       <c r="E32" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="F32" t="s">
-        <v>245</v>
-      </c>
-      <c r="G32" s="42" t="s">
-        <v>255</v>
+        <v>228</v>
+      </c>
+      <c r="G32" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="E33" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="F33" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="G33" t="s">
-        <v>208</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>243</v>
       </c>
       <c r="C34" t="s">
-        <v>249</v>
-      </c>
-      <c r="D34" t="s">
-        <v>250</v>
-      </c>
-      <c r="G34" s="47" t="s">
+        <v>255</v>
+      </c>
+      <c r="E34" t="s">
         <v>254</v>
+      </c>
+      <c r="F34" t="s">
+        <v>256</v>
+      </c>
+      <c r="G34" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>251</v>
+        <v>204</v>
       </c>
       <c r="F35" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="G35" t="s">
-        <v>252</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -2751,22 +2747,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
     </row>
@@ -2779,7 +2775,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>44259</v>
+        <v>44296</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2804,7 +2800,7 @@
       </c>
       <c r="B8" s="43" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2021-03-11</v>
+        <v>2021-04-17</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2813,7 +2809,7 @@
       </c>
       <c r="B9" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2021-03-15</v>
+        <v>2021-04-20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2822,7 +2818,7 @@
       </c>
       <c r="B10" s="44" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20210304</v>
+        <v>20210410</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2832,7 +2828,7 @@
       </c>
       <c r="B12" s="43" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2021-03-04</v>
+        <v>2021-04-10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,15 +2837,15 @@
       </c>
       <c r="B13" s="43" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2021-02-22</v>
+        <v>2021-03-29</v>
       </c>
       <c r="C13" s="43" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2021-02-26</v>
+        <v>2021-04-02</v>
       </c>
       <c r="D13" s="45" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2021-02-28</v>
+        <v>2021-04-04</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2858,11 +2854,11 @@
       </c>
       <c r="B14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
-        <v>2021-02-01</v>
+        <v>2021-03-01</v>
       </c>
       <c r="C14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
-        <v>2021-02-28</v>
+        <v>2021-03-31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2871,21 +2867,21 @@
       </c>
       <c r="B15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
-        <v>2021-03-01</v>
+        <v>2021-04-01</v>
       </c>
       <c r="C15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
-        <v>2021-03-31</v>
+        <v>2021-04-30</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -2899,11 +2895,11 @@
       <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="49" t="s">
+      <c r="B19" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -3073,24 +3069,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="25" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -3310,18 +3306,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
@@ -3368,10 +3364,10 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="53"/>
+      <c r="B9" s="51"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
@@ -3446,18 +3442,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
@@ -3468,10 +3464,10 @@
       <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="53"/>
+      <c r="B4" s="51"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">

</xml_diff>

<commit_message>
Update project and import AII prof info.
</commit_message>
<xml_diff>
--- a/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
+++ b/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMD\Documents\UiPath\Is prof extractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sako_\source\repos\data-import\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462EA7EF-9818-4DEC-9E45-782FDFC61839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD25C057-92F0-4808-8C80-1B32A37AD64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
-    <sheet name="Date" sheetId="1" r:id="rId2"/>
-    <sheet name="Text" sheetId="3" r:id="rId3"/>
-    <sheet name="Number" sheetId="4" r:id="rId4"/>
-    <sheet name="File" sheetId="5" r:id="rId5"/>
-    <sheet name="About the Project Notebook" sheetId="2" r:id="rId6"/>
+    <sheet name="Data" sheetId="7" r:id="rId1"/>
+    <sheet name="Scratchpad" sheetId="6" r:id="rId2"/>
+    <sheet name="Date" sheetId="1" r:id="rId3"/>
+    <sheet name="Text" sheetId="3" r:id="rId4"/>
+    <sheet name="Number" sheetId="4" r:id="rId5"/>
+    <sheet name="File" sheetId="5" r:id="rId6"/>
+    <sheet name="About the Project Notebook" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_A1">Scratchpad!$A$1</definedName>
@@ -64,17 +65,26 @@
     <definedName name="UpperCase">Text!$B$7</definedName>
     <definedName name="YYYYMMDD">Date!$B$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="265">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -846,6 +856,30 @@
   </si>
   <si>
     <t>/images/Poze_cadre_didactice/iulia_stamatescu.jpg</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>AII</t>
   </si>
 </sst>
 </file>
@@ -860,7 +894,7 @@
     <numFmt numFmtId="165" formatCode="yyyy;@"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,8 +1013,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,8 +1071,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1243,6 +1291,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1311,7 +1390,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1397,6 +1476,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1469,7 +1553,57 @@
     <cellStyle name="YellowCell 2" xfId="31" xr:uid="{982BBDC1-BDF7-4E08-B354-BEA94A3EC0BF}"/>
     <cellStyle name="z A Column text" xfId="7" xr:uid="{23B87D12-C661-428D-98E4-29837A850E3A}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1567,17 +1701,17 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CustomTableStyle" pivot="0" count="2" xr9:uid="{C0886BD5-2816-460A-9ABA-29A772184C96}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
     </tableStyle>
     <tableStyle name="ExcelTableStyle" pivot="0" count="7" xr9:uid="{1D1EB055-14F4-4341-8FDF-BB495A4C75BA}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1690,6 +1824,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A9ECB9E-3CCA-4091-B3EA-3340F1CF97FD}" name="Table1" displayName="Table1" ref="A1:G35" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:G35" xr:uid="{1A9ECB9E-3CCA-4091-B3EA-3340F1CF97FD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{45C2D8B1-3C51-4373-8699-FF65DF1DDE7C}" name="name">
+      <calculatedColumnFormula>PROPER(MID(Scratchpad!A2&amp;" "&amp;Scratchpad!A2,FIND(" ",Scratchpad!A2)+1,LEN(Scratchpad!A2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{370520B8-A3CB-4594-B2BB-5CE5044DA3B6}" name="office" dataDxfId="3">
+      <calculatedColumnFormula>Table2[[#This Row],[Birou]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C968511F-48B0-4416-BDCF-C6ECFF37E877}" name="position" dataDxfId="2">
+      <calculatedColumnFormula>Table2[[#This Row],[Titlu]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7DAD84E7-C83B-4E9E-B716-F72E3A8D3A5A}" name="phone"/>
+    <tableColumn id="5" xr3:uid="{28F195C8-74C5-47D3-B2C7-79764DFDEC9C}" name="photo" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{92DB11FC-50B7-44F6-8F32-066E3EF8CB0A}" name="email" dataDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[Email]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{61C8B0FC-EDB6-4A8B-966A-EEF9370D3743}" name="department"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E136979-B8AA-4BDC-8BEF-57C975F3020D}" name="Table2" displayName="Table2" ref="A1:G35" totalsRowShown="0">
   <autoFilter ref="A1:G35" xr:uid="{DEBA6575-C810-4844-8160-17F8B7FB45E0}"/>
   <tableColumns count="7">
@@ -2001,26 +2161,925 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF50CED-C8F1-4F66-BAB7-4A5C12533653}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>PROPER(MID(Scratchpad!A2&amp;" "&amp;Scratchpad!A2,FIND(" ",Scratchpad!A2)+1,LEN(Scratchpad!A2)))</f>
+        <v>Ana Magdalena Anghel</v>
+      </c>
+      <c r="B2" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED410</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anghel_magda.jpg</v>
+      </c>
+      <c r="F2" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ana.anghel@upb.ro</v>
+      </c>
+      <c r="G2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A3&amp;" "&amp;Scratchpad!A3,FIND(" ",Scratchpad!A3)+1,LEN(Scratchpad!A3)))</f>
+        <v>Florin Anton</v>
+      </c>
+      <c r="B3" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED309</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anton_florin.jpg</v>
+      </c>
+      <c r="F3" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>florin.anton@upb.ro</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A4&amp;" "&amp;Scratchpad!A4,FIND(" ",Scratchpad!A4)+1,LEN(Scratchpad!A4)))</f>
+        <v>Silvia Anton</v>
+      </c>
+      <c r="B4" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E4" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anton_silvia.jpg</v>
+      </c>
+      <c r="F4" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>silvia.anton@upb.ro</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A5&amp;" "&amp;Scratchpad!A5,FIND(" ",Scratchpad!A5)+1,LEN(Scratchpad!A5)))</f>
+        <v>Nicoleta Arghira</v>
+      </c>
+      <c r="B5" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212/PR406</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E5" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/arghira_nicoleta.jpg</v>
+      </c>
+      <c r="F5" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>nicoleta.arghira@upb.ro</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A6&amp;" "&amp;Scratchpad!A6,FIND(" ",Scratchpad!A6)+1,LEN(Scratchpad!A6)))</f>
+        <v>Theodor Borangiu</v>
+      </c>
+      <c r="B6" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E6" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/borangiu_theodor.jpg</v>
+      </c>
+      <c r="F6" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>theodor.borangiu@upb.ro</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A7&amp;" "&amp;Scratchpad!A7,FIND(" ",Scratchpad!A7)+1,LEN(Scratchpad!A7)))</f>
+        <v>Vasile Calofir</v>
+      </c>
+      <c r="B7" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED115</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>SL dr.ing.</v>
+      </c>
+      <c r="E7" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/calofir_vasile.jpg</v>
+      </c>
+      <c r="F7" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>vasile.calofir@upb.ro</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A8&amp;" "&amp;Scratchpad!A8,FIND(" ",Scratchpad!A8)+1,LEN(Scratchpad!A8)))</f>
+        <v>Simona Iuliana Caramihai</v>
+      </c>
+      <c r="B8" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED209</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/caramihai_simona.jpg</v>
+      </c>
+      <c r="F8" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>simona.caramihai@upb.ro</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A9&amp;" "&amp;Scratchpad!A9,FIND(" ",Scratchpad!A9)+1,LEN(Scratchpad!A9)))</f>
+        <v>Alexandra Cernian</v>
+      </c>
+      <c r="B9" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E9" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/cernian_alexandra.jpg</v>
+      </c>
+      <c r="F9" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>alexandra.cernian@upb.ro</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A10&amp;" "&amp;Scratchpad!A10,FIND(" ",Scratchpad!A10)+1,LEN(Scratchpad!A10)))</f>
+        <v>Oana Gabriela Chenaru</v>
+      </c>
+      <c r="B10" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E10" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/chenaru_oana.jpg</v>
+      </c>
+      <c r="F10" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>oana.chenaru@upb.ro</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A11&amp;" "&amp;Scratchpad!A11,FIND(" ",Scratchpad!A11)+1,LEN(Scratchpad!A11)))</f>
+        <v>Radu Dobrescu</v>
+      </c>
+      <c r="B11" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305, PRECIS 403</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing., coordonator doctorat</v>
+      </c>
+      <c r="E11" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/radu_dobrescu.jpg</v>
+      </c>
+      <c r="F11" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>radu.dobrescu@upb.ro</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A12&amp;" "&amp;Scratchpad!A12,FIND(" ",Scratchpad!A12)+1,LEN(Scratchpad!A12)))</f>
+        <v>Liliana Dobrica</v>
+      </c>
+      <c r="B12" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E12" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/dobrica_liliana.jpg</v>
+      </c>
+      <c r="F12" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>liliana.dobrica@upb.ro</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A13&amp;" "&amp;Scratchpad!A13,FIND(" ",Scratchpad!A13)+1,LEN(Scratchpad!A13)))</f>
+        <v>Alexandru Dumitrache</v>
+      </c>
+      <c r="B13" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED413</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E13" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/dumitrache_alexandru.jpg</v>
+      </c>
+      <c r="F13" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>alexandru.dumitrache@upb.ro</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A14&amp;" "&amp;Scratchpad!A14,FIND(" ",Scratchpad!A14)+1,LEN(Scratchpad!A14)))</f>
+        <v>Ioana Fagarasan</v>
+      </c>
+      <c r="B14" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212/ PRECIS 406</v>
+      </c>
+      <c r="C14" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E14" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/fagarasan_ioana.jpg</v>
+      </c>
+      <c r="F14" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ioana.fagarasan@upb.ro</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A15&amp;" "&amp;Scratchpad!A15,FIND(" ",Scratchpad!A15)+1,LEN(Scratchpad!A15)))</f>
+        <v>Andrei Hossu</v>
+      </c>
+      <c r="B15" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED414</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E15" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/andrei_hossu.jpg</v>
+      </c>
+      <c r="F15" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>andrei.hossu@upb.ro</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A16&amp;" "&amp;Scratchpad!A16,FIND(" ",Scratchpad!A16)+1,LEN(Scratchpad!A16)))</f>
+        <v>Daniela Hossu</v>
+      </c>
+      <c r="B16" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E16" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F16" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniela.hossu@upb.ro</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A17&amp;" "&amp;Scratchpad!A17,FIND(" ",Scratchpad!A17)+1,LEN(Scratchpad!A17)))</f>
+        <v>Iulia-Lidia Iacob</v>
+      </c>
+      <c r="B17" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E17" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/iacob_lidia.jpg</v>
+      </c>
+      <c r="F17" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>iulia.iacob@upb.ro</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A18&amp;" "&amp;Scratchpad!A18,FIND(" ",Scratchpad!A18)+1,LEN(Scratchpad!A18)))</f>
+        <v>Loretta Ichim</v>
+      </c>
+      <c r="B18" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305/ PRECIS 403</v>
+      </c>
+      <c r="C18" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E18" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ichim_loretta.jpg</v>
+      </c>
+      <c r="F18" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>loretta.ichim@upb.ro</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A19&amp;" "&amp;Scratchpad!A19,FIND(" ",Scratchpad!A19)+1,LEN(Scratchpad!A19)))</f>
+        <v>Anca Daniela Ionita</v>
+      </c>
+      <c r="B19" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415, PRECIS 401</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E19" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ionita_anca_2.jpg</v>
+      </c>
+      <c r="F19" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>anca.ionita@upb.ro</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A20&amp;" "&amp;Scratchpad!A20,FIND(" ",Scratchpad!A20)+1,LEN(Scratchpad!A20)))</f>
+        <v>Andrei Nik Ivanescu</v>
+      </c>
+      <c r="B20" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C20" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E20" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ivanescu_nick.jpg</v>
+      </c>
+      <c r="F20" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>nik.ivanescu@upb.ro</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A21&amp;" "&amp;Scratchpad!A21,FIND(" ",Scratchpad!A21)+1,LEN(Scratchpad!A21)))</f>
+        <v>Daniel Marian Merezeanu</v>
+      </c>
+      <c r="B21" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E21" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/merezeanu_daniel.jpg</v>
+      </c>
+      <c r="F21" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniel.merezeanu@upb.ro</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A22&amp;" "&amp;Scratchpad!A22,FIND(" ",Scratchpad!A22)+1,LEN(Scratchpad!A22)))</f>
+        <v>Stefan Alexandru Mocanu</v>
+      </c>
+      <c r="B22" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C22" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E22" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/st_moc.jpg</v>
+      </c>
+      <c r="F22" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>stefan.mocanu@upb.ro</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A23&amp;" "&amp;Scratchpad!A23,FIND(" ",Scratchpad!A23)+1,LEN(Scratchpad!A23)))</f>
+        <v>Mihnea Alexandru Moisescu</v>
+      </c>
+      <c r="B23" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED209-210</v>
+      </c>
+      <c r="C23" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E23" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/moisescu_mihnea.jpg</v>
+      </c>
+      <c r="F23" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>mihnea.moisescu@upb.ro</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A24&amp;" "&amp;Scratchpad!A24,FIND(" ",Scratchpad!A24)+1,LEN(Scratchpad!A24)))</f>
+        <v>Cristina Nichiforov</v>
+      </c>
+      <c r="B24" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED211-212</v>
+      </c>
+      <c r="C24" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>As. dr.ing.</v>
+      </c>
+      <c r="E24" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/nichiforov_cristina.jpg</v>
+      </c>
+      <c r="F24" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>cristina.nichiforov@upb.ro</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A25&amp;" "&amp;Scratchpad!A25,FIND(" ",Scratchpad!A25)+1,LEN(Scratchpad!A25)))</f>
+        <v>Maximilian Eugen Nicolae</v>
+      </c>
+      <c r="B25" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C25" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E25" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/nicolae_maximilian.jpg</v>
+      </c>
+      <c r="F25" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>max.nicolae@upb.ro</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A26&amp;" "&amp;Scratchpad!A26,FIND(" ",Scratchpad!A26)+1,LEN(Scratchpad!A26)))</f>
+        <v>Virginia Ecaterina Oltean</v>
+      </c>
+      <c r="B26" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C26" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E26" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F26" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ecaterina.oltean@upb.ro</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A27&amp;" "&amp;Scratchpad!A27,FIND(" ",Scratchpad!A27)+1,LEN(Scratchpad!A27)))</f>
+        <v>Adriana Olteanu</v>
+      </c>
+      <c r="B27" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E27" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/olteanu_adriana.jpg</v>
+      </c>
+      <c r="F27" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>adriana.olteanu@upb.ro</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A28&amp;" "&amp;Scratchpad!A28,FIND(" ",Scratchpad!A28)+1,LEN(Scratchpad!A28)))</f>
+        <v>Radu Nicolae Pietraru</v>
+      </c>
+      <c r="B28" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED413</v>
+      </c>
+      <c r="C28" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E28" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/pietraru_radu.jpg</v>
+      </c>
+      <c r="F28" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>radu.pietraru@upb.ro</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A29&amp;" "&amp;Scratchpad!A29,FIND(" ",Scratchpad!A29)+1,LEN(Scratchpad!A29)))</f>
+        <v>Dan Popescu</v>
+      </c>
+      <c r="B29" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305, PRECIS 403</v>
+      </c>
+      <c r="C29" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E29" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/popescu_dan.jpg</v>
+      </c>
+      <c r="F29" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>dan.popescu@upb.ro</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A30&amp;" "&amp;Scratchpad!A30,FIND(" ",Scratchpad!A30)+1,LEN(Scratchpad!A30)))</f>
+        <v>Silviu Raileanu</v>
+      </c>
+      <c r="B30" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C30" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E30" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/raileanu_silviu.jpg</v>
+      </c>
+      <c r="F30" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>silviu.raileanu@upb.ro</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A31&amp;" "&amp;Scratchpad!A31,FIND(" ",Scratchpad!A31)+1,LEN(Scratchpad!A31)))</f>
+        <v>Daniela Saru</v>
+      </c>
+      <c r="B31" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED406</v>
+      </c>
+      <c r="C31" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E31" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/saru_daniela.jpg</v>
+      </c>
+      <c r="F31" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniela.saru@upb.ro</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A32&amp;" "&amp;Scratchpad!A32,FIND(" ",Scratchpad!A32)+1,LEN(Scratchpad!A32)))</f>
+        <v>Mircea Stefan Simoiu</v>
+      </c>
+      <c r="B32" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212</v>
+      </c>
+      <c r="C32" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>As. drd.ing.</v>
+      </c>
+      <c r="E32" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F32" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>mircea_stefan.simoiu@upb.ro</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A33&amp;" "&amp;Scratchpad!A33,FIND(" ",Scratchpad!A33)+1,LEN(Scratchpad!A33)))</f>
+        <v>Grigore Stamatescu</v>
+      </c>
+      <c r="B33" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>PRECIS 406</v>
+      </c>
+      <c r="C33" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E33" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/stamatescu_grigore.jpg</v>
+      </c>
+      <c r="F33" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>grigore.stamatescu@upb.ro</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A34&amp;" "&amp;Scratchpad!A34,FIND(" ",Scratchpad!A34)+1,LEN(Scratchpad!A34)))</f>
+        <v>Iulia Vasilica Stamatescu</v>
+      </c>
+      <c r="B34" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED213/ PRECIS 406</v>
+      </c>
+      <c r="C34" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E34" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/iulia_stamatescu.jpg</v>
+      </c>
+      <c r="F34" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>iulia.stamatescu@upb.ro</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A35&amp;" "&amp;Scratchpad!A35,FIND(" ",Scratchpad!A35)+1,LEN(Scratchpad!A35)))</f>
+        <v>Madalin Vlad</v>
+      </c>
+      <c r="B35" s="50">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>0</v>
+      </c>
+      <c r="C35" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>SL dr.ing.</v>
+      </c>
+      <c r="E35" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F35" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>madalin.vlad@upb.ro</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="48.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="48.26953125" customWidth="1"/>
+    <col min="7" max="7" width="37.453125" customWidth="1"/>
+    <col min="8" max="8" width="27.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2043,7 +3102,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -2063,7 +3122,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2083,7 +3142,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -2103,7 +3162,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2123,7 +3182,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -2143,7 +3202,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -2163,7 +3222,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -2183,7 +3242,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -2203,7 +3262,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -2223,7 +3282,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -2243,7 +3302,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -2263,7 +3322,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2283,7 +3342,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -2303,7 +3362,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>236</v>
       </c>
@@ -2323,7 +3382,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -2343,7 +3402,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -2363,7 +3422,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -2383,7 +3442,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -2403,7 +3462,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -2423,7 +3482,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -2443,7 +3502,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>240</v>
       </c>
@@ -2463,7 +3522,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2483,7 +3542,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -2503,7 +3562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -2523,7 +3582,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -2543,7 +3602,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2563,7 +3622,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -2583,7 +3642,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2603,7 +3662,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2623,7 +3682,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2643,7 +3702,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -2663,7 +3722,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2683,7 +3742,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>242</v>
       </c>
@@ -2703,7 +3762,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -2729,7 +3788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -2737,48 +3796,48 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="4" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>44296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>84</v>
       </c>
@@ -2786,7 +3845,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>58</v>
       </c>
@@ -2794,96 +3853,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="43" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2021-04-17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2021-08-03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2021-04-20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-08-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="44" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20210410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20210727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="43" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2021-04-10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-07-27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="43" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2021-03-29</v>
+        <v>2021-07-19</v>
       </c>
       <c r="C13" s="43" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2021-04-02</v>
+        <v>2021-07-23</v>
       </c>
       <c r="D13" s="45" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2021-04-04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-07-25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
-        <v>2021-03-01</v>
+        <v>2021-06-01</v>
       </c>
       <c r="C14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
-        <v>2021-03-31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-06-30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
-        <v>2021-04-01</v>
+        <v>2021-07-01</v>
       </c>
       <c r="C15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
-        <v>2021-04-30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49" t="s">
+        <v>2021-07-30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2891,17 +3950,17 @@
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
@@ -2915,7 +3974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
@@ -2925,7 +3984,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
@@ -2933,7 +3992,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>28</v>
       </c>
@@ -2950,7 +4009,7 @@
         <v>12月31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
@@ -2961,7 +4020,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -2972,7 +4031,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2987,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>32</v>
       </c>
@@ -2998,7 +4057,7 @@
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>33</v>
       </c>
@@ -3009,7 +4068,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>22</v>
       </c>
@@ -3017,7 +4076,7 @@
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="46" t="s">
         <v>86</v>
       </c>
@@ -3028,7 +4087,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
@@ -3051,7 +4110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7C60E3-5132-4EAF-A6AE-357FE13BC6C9}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -3059,36 +4118,36 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3108,7 +4167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3130,7 +4189,7 @@
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3150,7 +4209,7 @@
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3170,7 +4229,7 @@
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3190,7 +4249,7 @@
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>64</v>
       </c>
@@ -3199,7 +4258,7 @@
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3210,7 +4269,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3221,7 +4280,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3233,7 +4292,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3245,12 +4304,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -3262,7 +4321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3274,7 +4333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>64</v>
       </c>
@@ -3289,7 +4348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C83CC8-3284-4752-8E92-8CBBD1003835}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -3297,37 +4356,37 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -3335,7 +4394,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>68</v>
       </c>
@@ -3344,7 +4403,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3353,7 +4412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3362,20 +4421,20 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="51"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -3383,7 +4442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +4451,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
@@ -3400,13 +4459,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
@@ -3426,7 +4485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -3434,48 +4493,48 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.140625" customWidth="1"/>
+    <col min="3" max="4" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="51"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
@@ -3483,13 +4542,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="17"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
@@ -3498,7 +4557,7 @@
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>42</v>
       </c>
@@ -3507,7 +4566,7 @@
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>41</v>
       </c>
@@ -3516,7 +4575,7 @@
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
         <v>56</v>
       </c>
@@ -3525,7 +4584,7 @@
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>57</v>
       </c>
@@ -3544,122 +4603,122 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="165.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="30"/>
+    <col min="1" max="1" width="165.54296875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36"/>
     </row>
-    <row r="2" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="35"/>
       <c r="D4" s="31"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="35"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="35"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="35"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="35"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="35"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="35"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="35"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="35"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="35"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="35"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="37" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="37" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Update project and import AII prof info. (#7)
* Update dependencies.

* Update project and import AII prof info.

* Remove config.json.

* Remove firebase-admin.
</commit_message>
<xml_diff>
--- a/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
+++ b/crawlers/UiPath StudioX/IS_prof_extractor/Project_Notebook.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMD\Documents\UiPath\Is prof extractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sako_\source\repos\data-import\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462EA7EF-9818-4DEC-9E45-782FDFC61839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD25C057-92F0-4808-8C80-1B32A37AD64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CEA043F9-B9CC-4A62-BD5F-6FF44D9B0F3D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Scratchpad" sheetId="6" r:id="rId1"/>
-    <sheet name="Date" sheetId="1" r:id="rId2"/>
-    <sheet name="Text" sheetId="3" r:id="rId3"/>
-    <sheet name="Number" sheetId="4" r:id="rId4"/>
-    <sheet name="File" sheetId="5" r:id="rId5"/>
-    <sheet name="About the Project Notebook" sheetId="2" r:id="rId6"/>
+    <sheet name="Data" sheetId="7" r:id="rId1"/>
+    <sheet name="Scratchpad" sheetId="6" r:id="rId2"/>
+    <sheet name="Date" sheetId="1" r:id="rId3"/>
+    <sheet name="Text" sheetId="3" r:id="rId4"/>
+    <sheet name="Number" sheetId="4" r:id="rId5"/>
+    <sheet name="File" sheetId="5" r:id="rId6"/>
+    <sheet name="About the Project Notebook" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_A1">Scratchpad!$A$1</definedName>
@@ -64,17 +65,26 @@
     <definedName name="UpperCase">Text!$B$7</definedName>
     <definedName name="YYYYMMDD">Date!$B$10</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="265">
   <si>
     <t>Last month's dates (First and Last)</t>
   </si>
@@ -846,6 +856,30 @@
   </si>
   <si>
     <t>/images/Poze_cadre_didactice/iulia_stamatescu.jpg</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>AII</t>
   </si>
 </sst>
 </file>
@@ -860,7 +894,7 @@
     <numFmt numFmtId="165" formatCode="yyyy;@"/>
     <numFmt numFmtId="166" formatCode="dd\-mmm"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,8 +1013,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,8 +1071,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1243,6 +1291,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1311,7 +1390,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1397,6 +1476,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1469,7 +1553,57 @@
     <cellStyle name="YellowCell 2" xfId="31" xr:uid="{982BBDC1-BDF7-4E08-B354-BEA94A3EC0BF}"/>
     <cellStyle name="z A Column text" xfId="7" xr:uid="{23B87D12-C661-428D-98E4-29837A850E3A}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="16">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1567,17 +1701,17 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CustomTableStyle" pivot="0" count="2" xr9:uid="{C0886BD5-2816-460A-9ABA-29A772184C96}">
-      <tableStyleElement type="headerRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
     </tableStyle>
     <tableStyle name="ExcelTableStyle" pivot="0" count="7" xr9:uid="{1D1EB055-14F4-4341-8FDF-BB495A4C75BA}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1690,6 +1824,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A9ECB9E-3CCA-4091-B3EA-3340F1CF97FD}" name="Table1" displayName="Table1" ref="A1:G35" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:G35" xr:uid="{1A9ECB9E-3CCA-4091-B3EA-3340F1CF97FD}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{45C2D8B1-3C51-4373-8699-FF65DF1DDE7C}" name="name">
+      <calculatedColumnFormula>PROPER(MID(Scratchpad!A2&amp;" "&amp;Scratchpad!A2,FIND(" ",Scratchpad!A2)+1,LEN(Scratchpad!A2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{370520B8-A3CB-4594-B2BB-5CE5044DA3B6}" name="office" dataDxfId="3">
+      <calculatedColumnFormula>Table2[[#This Row],[Birou]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C968511F-48B0-4416-BDCF-C6ECFF37E877}" name="position" dataDxfId="2">
+      <calculatedColumnFormula>Table2[[#This Row],[Titlu]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{7DAD84E7-C83B-4E9E-B716-F72E3A8D3A5A}" name="phone"/>
+    <tableColumn id="5" xr3:uid="{28F195C8-74C5-47D3-B2C7-79764DFDEC9C}" name="photo" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{92DB11FC-50B7-44F6-8F32-066E3EF8CB0A}" name="email" dataDxfId="0">
+      <calculatedColumnFormula>Table2[[#This Row],[Email]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{61C8B0FC-EDB6-4A8B-966A-EEF9370D3743}" name="department"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5E136979-B8AA-4BDC-8BEF-57C975F3020D}" name="Table2" displayName="Table2" ref="A1:G35" totalsRowShown="0">
   <autoFilter ref="A1:G35" xr:uid="{DEBA6575-C810-4844-8160-17F8B7FB45E0}"/>
   <tableColumns count="7">
@@ -2001,26 +2161,925 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF50CED-C8F1-4F66-BAB7-4A5C12533653}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>259</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="str">
+        <f>PROPER(MID(Scratchpad!A2&amp;" "&amp;Scratchpad!A2,FIND(" ",Scratchpad!A2)+1,LEN(Scratchpad!A2)))</f>
+        <v>Ana Magdalena Anghel</v>
+      </c>
+      <c r="B2" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED410</v>
+      </c>
+      <c r="C2" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E2" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anghel_magda.jpg</v>
+      </c>
+      <c r="F2" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ana.anghel@upb.ro</v>
+      </c>
+      <c r="G2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A3&amp;" "&amp;Scratchpad!A3,FIND(" ",Scratchpad!A3)+1,LEN(Scratchpad!A3)))</f>
+        <v>Florin Anton</v>
+      </c>
+      <c r="B3" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED309</v>
+      </c>
+      <c r="C3" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anton_florin.jpg</v>
+      </c>
+      <c r="F3" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>florin.anton@upb.ro</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A4&amp;" "&amp;Scratchpad!A4,FIND(" ",Scratchpad!A4)+1,LEN(Scratchpad!A4)))</f>
+        <v>Silvia Anton</v>
+      </c>
+      <c r="B4" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E4" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/anton_silvia.jpg</v>
+      </c>
+      <c r="F4" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>silvia.anton@upb.ro</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A5&amp;" "&amp;Scratchpad!A5,FIND(" ",Scratchpad!A5)+1,LEN(Scratchpad!A5)))</f>
+        <v>Nicoleta Arghira</v>
+      </c>
+      <c r="B5" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212/PR406</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E5" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/arghira_nicoleta.jpg</v>
+      </c>
+      <c r="F5" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>nicoleta.arghira@upb.ro</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A6&amp;" "&amp;Scratchpad!A6,FIND(" ",Scratchpad!A6)+1,LEN(Scratchpad!A6)))</f>
+        <v>Theodor Borangiu</v>
+      </c>
+      <c r="B6" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E6" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/borangiu_theodor.jpg</v>
+      </c>
+      <c r="F6" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>theodor.borangiu@upb.ro</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A7&amp;" "&amp;Scratchpad!A7,FIND(" ",Scratchpad!A7)+1,LEN(Scratchpad!A7)))</f>
+        <v>Vasile Calofir</v>
+      </c>
+      <c r="B7" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED115</v>
+      </c>
+      <c r="C7" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>SL dr.ing.</v>
+      </c>
+      <c r="E7" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/calofir_vasile.jpg</v>
+      </c>
+      <c r="F7" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>vasile.calofir@upb.ro</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A8&amp;" "&amp;Scratchpad!A8,FIND(" ",Scratchpad!A8)+1,LEN(Scratchpad!A8)))</f>
+        <v>Simona Iuliana Caramihai</v>
+      </c>
+      <c r="B8" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED209</v>
+      </c>
+      <c r="C8" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/caramihai_simona.jpg</v>
+      </c>
+      <c r="F8" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>simona.caramihai@upb.ro</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A9&amp;" "&amp;Scratchpad!A9,FIND(" ",Scratchpad!A9)+1,LEN(Scratchpad!A9)))</f>
+        <v>Alexandra Cernian</v>
+      </c>
+      <c r="B9" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C9" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E9" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/cernian_alexandra.jpg</v>
+      </c>
+      <c r="F9" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>alexandra.cernian@upb.ro</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A10&amp;" "&amp;Scratchpad!A10,FIND(" ",Scratchpad!A10)+1,LEN(Scratchpad!A10)))</f>
+        <v>Oana Gabriela Chenaru</v>
+      </c>
+      <c r="B10" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C10" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E10" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/chenaru_oana.jpg</v>
+      </c>
+      <c r="F10" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>oana.chenaru@upb.ro</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A11&amp;" "&amp;Scratchpad!A11,FIND(" ",Scratchpad!A11)+1,LEN(Scratchpad!A11)))</f>
+        <v>Radu Dobrescu</v>
+      </c>
+      <c r="B11" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305, PRECIS 403</v>
+      </c>
+      <c r="C11" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing., coordonator doctorat</v>
+      </c>
+      <c r="E11" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/radu_dobrescu.jpg</v>
+      </c>
+      <c r="F11" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>radu.dobrescu@upb.ro</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A12&amp;" "&amp;Scratchpad!A12,FIND(" ",Scratchpad!A12)+1,LEN(Scratchpad!A12)))</f>
+        <v>Liliana Dobrica</v>
+      </c>
+      <c r="B12" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C12" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E12" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/dobrica_liliana.jpg</v>
+      </c>
+      <c r="F12" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>liliana.dobrica@upb.ro</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A13&amp;" "&amp;Scratchpad!A13,FIND(" ",Scratchpad!A13)+1,LEN(Scratchpad!A13)))</f>
+        <v>Alexandru Dumitrache</v>
+      </c>
+      <c r="B13" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED413</v>
+      </c>
+      <c r="C13" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E13" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/dumitrache_alexandru.jpg</v>
+      </c>
+      <c r="F13" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>alexandru.dumitrache@upb.ro</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A14&amp;" "&amp;Scratchpad!A14,FIND(" ",Scratchpad!A14)+1,LEN(Scratchpad!A14)))</f>
+        <v>Ioana Fagarasan</v>
+      </c>
+      <c r="B14" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212/ PRECIS 406</v>
+      </c>
+      <c r="C14" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E14" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/fagarasan_ioana.jpg</v>
+      </c>
+      <c r="F14" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ioana.fagarasan@upb.ro</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A15&amp;" "&amp;Scratchpad!A15,FIND(" ",Scratchpad!A15)+1,LEN(Scratchpad!A15)))</f>
+        <v>Andrei Hossu</v>
+      </c>
+      <c r="B15" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED414</v>
+      </c>
+      <c r="C15" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E15" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/andrei_hossu.jpg</v>
+      </c>
+      <c r="F15" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>andrei.hossu@upb.ro</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A16&amp;" "&amp;Scratchpad!A16,FIND(" ",Scratchpad!A16)+1,LEN(Scratchpad!A16)))</f>
+        <v>Daniela Hossu</v>
+      </c>
+      <c r="B16" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C16" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E16" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F16" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniela.hossu@upb.ro</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A17&amp;" "&amp;Scratchpad!A17,FIND(" ",Scratchpad!A17)+1,LEN(Scratchpad!A17)))</f>
+        <v>Iulia-Lidia Iacob</v>
+      </c>
+      <c r="B17" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C17" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E17" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/iacob_lidia.jpg</v>
+      </c>
+      <c r="F17" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>iulia.iacob@upb.ro</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A18&amp;" "&amp;Scratchpad!A18,FIND(" ",Scratchpad!A18)+1,LEN(Scratchpad!A18)))</f>
+        <v>Loretta Ichim</v>
+      </c>
+      <c r="B18" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305/ PRECIS 403</v>
+      </c>
+      <c r="C18" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E18" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ichim_loretta.jpg</v>
+      </c>
+      <c r="F18" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>loretta.ichim@upb.ro</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A19&amp;" "&amp;Scratchpad!A19,FIND(" ",Scratchpad!A19)+1,LEN(Scratchpad!A19)))</f>
+        <v>Anca Daniela Ionita</v>
+      </c>
+      <c r="B19" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415, PRECIS 401</v>
+      </c>
+      <c r="C19" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E19" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ionita_anca_2.jpg</v>
+      </c>
+      <c r="F19" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>anca.ionita@upb.ro</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A20&amp;" "&amp;Scratchpad!A20,FIND(" ",Scratchpad!A20)+1,LEN(Scratchpad!A20)))</f>
+        <v>Andrei Nik Ivanescu</v>
+      </c>
+      <c r="B20" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C20" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E20" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/ivanescu_nick.jpg</v>
+      </c>
+      <c r="F20" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>nik.ivanescu@upb.ro</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A21&amp;" "&amp;Scratchpad!A21,FIND(" ",Scratchpad!A21)+1,LEN(Scratchpad!A21)))</f>
+        <v>Daniel Marian Merezeanu</v>
+      </c>
+      <c r="B21" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305</v>
+      </c>
+      <c r="C21" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E21" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/merezeanu_daniel.jpg</v>
+      </c>
+      <c r="F21" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniel.merezeanu@upb.ro</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A22&amp;" "&amp;Scratchpad!A22,FIND(" ",Scratchpad!A22)+1,LEN(Scratchpad!A22)))</f>
+        <v>Stefan Alexandru Mocanu</v>
+      </c>
+      <c r="B22" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C22" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E22" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/st_moc.jpg</v>
+      </c>
+      <c r="F22" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>stefan.mocanu@upb.ro</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A23&amp;" "&amp;Scratchpad!A23,FIND(" ",Scratchpad!A23)+1,LEN(Scratchpad!A23)))</f>
+        <v>Mihnea Alexandru Moisescu</v>
+      </c>
+      <c r="B23" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED209-210</v>
+      </c>
+      <c r="C23" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E23" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/moisescu_mihnea.jpg</v>
+      </c>
+      <c r="F23" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>mihnea.moisescu@upb.ro</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A24&amp;" "&amp;Scratchpad!A24,FIND(" ",Scratchpad!A24)+1,LEN(Scratchpad!A24)))</f>
+        <v>Cristina Nichiforov</v>
+      </c>
+      <c r="B24" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED211-212</v>
+      </c>
+      <c r="C24" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>As. dr.ing.</v>
+      </c>
+      <c r="E24" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/nichiforov_cristina.jpg</v>
+      </c>
+      <c r="F24" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>cristina.nichiforov@upb.ro</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A25&amp;" "&amp;Scratchpad!A25,FIND(" ",Scratchpad!A25)+1,LEN(Scratchpad!A25)))</f>
+        <v>Maximilian Eugen Nicolae</v>
+      </c>
+      <c r="B25" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED303</v>
+      </c>
+      <c r="C25" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E25" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/nicolae_maximilian.jpg</v>
+      </c>
+      <c r="F25" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>max.nicolae@upb.ro</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A26&amp;" "&amp;Scratchpad!A26,FIND(" ",Scratchpad!A26)+1,LEN(Scratchpad!A26)))</f>
+        <v>Virginia Ecaterina Oltean</v>
+      </c>
+      <c r="B26" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C26" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E26" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F26" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>ecaterina.oltean@upb.ro</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A27&amp;" "&amp;Scratchpad!A27,FIND(" ",Scratchpad!A27)+1,LEN(Scratchpad!A27)))</f>
+        <v>Adriana Olteanu</v>
+      </c>
+      <c r="B27" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED415</v>
+      </c>
+      <c r="C27" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E27" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/olteanu_adriana.jpg</v>
+      </c>
+      <c r="F27" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>adriana.olteanu@upb.ro</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A28&amp;" "&amp;Scratchpad!A28,FIND(" ",Scratchpad!A28)+1,LEN(Scratchpad!A28)))</f>
+        <v>Radu Nicolae Pietraru</v>
+      </c>
+      <c r="B28" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED413</v>
+      </c>
+      <c r="C28" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Sef lucrari dr.ing.</v>
+      </c>
+      <c r="E28" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/pietraru_radu.jpg</v>
+      </c>
+      <c r="F28" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>radu.pietraru@upb.ro</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A29&amp;" "&amp;Scratchpad!A29,FIND(" ",Scratchpad!A29)+1,LEN(Scratchpad!A29)))</f>
+        <v>Dan Popescu</v>
+      </c>
+      <c r="B29" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED305, PRECIS 403</v>
+      </c>
+      <c r="C29" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E29" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/popescu_dan.jpg</v>
+      </c>
+      <c r="F29" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>dan.popescu@upb.ro</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A30&amp;" "&amp;Scratchpad!A30,FIND(" ",Scratchpad!A30)+1,LEN(Scratchpad!A30)))</f>
+        <v>Silviu Raileanu</v>
+      </c>
+      <c r="B30" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED111</v>
+      </c>
+      <c r="C30" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E30" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/raileanu_silviu.jpg</v>
+      </c>
+      <c r="F30" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>silviu.raileanu@upb.ro</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A31&amp;" "&amp;Scratchpad!A31,FIND(" ",Scratchpad!A31)+1,LEN(Scratchpad!A31)))</f>
+        <v>Daniela Saru</v>
+      </c>
+      <c r="B31" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED406</v>
+      </c>
+      <c r="C31" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Profesor dr.ing.</v>
+      </c>
+      <c r="E31" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/saru_daniela.jpg</v>
+      </c>
+      <c r="F31" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>daniela.saru@upb.ro</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A32&amp;" "&amp;Scratchpad!A32,FIND(" ",Scratchpad!A32)+1,LEN(Scratchpad!A32)))</f>
+        <v>Mircea Stefan Simoiu</v>
+      </c>
+      <c r="B32" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED212</v>
+      </c>
+      <c r="C32" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>As. drd.ing.</v>
+      </c>
+      <c r="E32" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F32" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>mircea_stefan.simoiu@upb.ro</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A33&amp;" "&amp;Scratchpad!A33,FIND(" ",Scratchpad!A33)+1,LEN(Scratchpad!A33)))</f>
+        <v>Grigore Stamatescu</v>
+      </c>
+      <c r="B33" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>PRECIS 406</v>
+      </c>
+      <c r="C33" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Educatie</v>
+      </c>
+      <c r="E33" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/stamatescu_grigore.jpg</v>
+      </c>
+      <c r="F33" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>grigore.stamatescu@upb.ro</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A34&amp;" "&amp;Scratchpad!A34,FIND(" ",Scratchpad!A34)+1,LEN(Scratchpad!A34)))</f>
+        <v>Iulia Vasilica Stamatescu</v>
+      </c>
+      <c r="B34" s="50" t="str">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>ED213/ PRECIS 406</v>
+      </c>
+      <c r="C34" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>Conferentiar dr.ing.</v>
+      </c>
+      <c r="E34" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/iulia_stamatescu.jpg</v>
+      </c>
+      <c r="F34" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>iulia.stamatescu@upb.ro</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="25" t="str">
+        <f>PROPER(MID(Scratchpad!A35&amp;" "&amp;Scratchpad!A35,FIND(" ",Scratchpad!A35)+1,LEN(Scratchpad!A35)))</f>
+        <v>Madalin Vlad</v>
+      </c>
+      <c r="B35" s="50">
+        <f>Table2[[#This Row],[Birou]]</f>
+        <v>0</v>
+      </c>
+      <c r="C35" t="str">
+        <f>Table2[[#This Row],[Titlu]]</f>
+        <v>SL dr.ing.</v>
+      </c>
+      <c r="E35" t="str">
+        <f>CONCATENATE("https://www.aii.pub.ro", Table2[[#This Row],[Poza]])</f>
+        <v>https://www.aii.pub.ro/images/Poze_cadre_didactice/zzz.jpg</v>
+      </c>
+      <c r="F35" t="str">
+        <f>Table2[[#This Row],[Email]]</f>
+        <v>madalin.vlad@upb.ro</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95188A8B-20B9-44C0-8B2D-2363D0E3925F}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.7265625" customWidth="1"/>
+    <col min="2" max="2" width="23.54296875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="48.28515625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="48.26953125" customWidth="1"/>
+    <col min="7" max="7" width="37.453125" customWidth="1"/>
+    <col min="8" max="8" width="27.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2043,7 +3102,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -2063,7 +3122,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -2083,7 +3142,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -2103,7 +3162,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -2123,7 +3182,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -2143,7 +3202,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -2163,7 +3222,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -2183,7 +3242,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -2203,7 +3262,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -2223,7 +3282,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -2243,7 +3302,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>98</v>
       </c>
@@ -2263,7 +3322,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2283,7 +3342,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -2303,7 +3362,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>236</v>
       </c>
@@ -2323,7 +3382,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>238</v>
       </c>
@@ -2343,7 +3402,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>101</v>
       </c>
@@ -2363,7 +3422,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>102</v>
       </c>
@@ -2383,7 +3442,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>103</v>
       </c>
@@ -2403,7 +3462,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>104</v>
       </c>
@@ -2423,7 +3482,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>105</v>
       </c>
@@ -2443,7 +3502,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>240</v>
       </c>
@@ -2463,7 +3522,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2483,7 +3542,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -2503,7 +3562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -2523,7 +3582,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -2543,7 +3602,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2563,7 +3622,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -2583,7 +3642,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2603,7 +3662,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>113</v>
       </c>
@@ -2623,7 +3682,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2643,7 +3702,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>115</v>
       </c>
@@ -2663,7 +3722,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -2683,7 +3742,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>242</v>
       </c>
@@ -2703,7 +3762,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>117</v>
       </c>
@@ -2729,7 +3788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53392D88-1157-4343-9701-AA198E0565D5}">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -2737,48 +3796,48 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="4" width="12.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
       <c r="E1" s="42"/>
       <c r="F1" s="42"/>
     </row>
-    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:6" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="42"/>
       <c r="F2" s="42"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2">
         <f ca="1">TODAY()</f>
-        <v>44296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+        <v>44404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
         <v>84</v>
       </c>
@@ -2786,7 +3845,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>58</v>
       </c>
@@ -2794,96 +3853,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="43" t="str">
         <f ca="1">TEXT(Date_Input+Days, preferred_date_format)</f>
-        <v>2021-04-17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2021-08-03</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B9" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(Date_Input, Days),preferred_date_format)</f>
-        <v>2021-04-20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-08-05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="44" t="str">
         <f ca="1">TEXT(Date_Input,"YYYYMMDD")</f>
-        <v>20210410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20210727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="43" t="str">
         <f ca="1">TEXT(TODAY(), preferred_date_format)</f>
-        <v>2021-04-10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-07-27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="43" t="str">
         <f ca="1">TEXT(TODAY()-WEEKDAY(TODAY(),2)-6, preferred_date_format)</f>
-        <v>2021-03-29</v>
+        <v>2021-07-19</v>
       </c>
       <c r="C13" s="43" t="str">
         <f ca="1">TEXT(LastWeekMonday+4, preferred_date_format)</f>
-        <v>2021-04-02</v>
+        <v>2021-07-23</v>
       </c>
       <c r="D13" s="45" t="str">
         <f ca="1">TEXT(LastWeekFriday+2, preferred_date_format)</f>
-        <v>2021-04-04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-07-25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY())-1, 1), preferred_date_format)</f>
-        <v>2021-03-01</v>
+        <v>2021-06-01</v>
       </c>
       <c r="C14" s="43" t="str">
         <f ca="1">TEXT(DATE(YEAR(TODAY()), MONTH(TODAY()), 0), preferred_date_format)</f>
-        <v>2021-03-31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2021-06-30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY()),1)-1,1), preferred_date_format)</f>
-        <v>2021-04-01</v>
+        <v>2021-07-01</v>
       </c>
       <c r="C15" s="43" t="str">
         <f ca="1">TEXT(WORKDAY(DATE(YEAR(TODAY()),MONTH(TODAY())+1,1),-1), preferred_date_format)</f>
-        <v>2021-04-30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49" t="s">
+        <v>2021-07-30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="51"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>19</v>
       </c>
@@ -2891,17 +3950,17 @@
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="52"/>
+      <c r="D19" s="53"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>23</v>
       </c>
@@ -2915,7 +3974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
@@ -2925,7 +3984,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
@@ -2933,7 +3992,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>28</v>
       </c>
@@ -2950,7 +4009,7 @@
         <v>12月31</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>29</v>
       </c>
@@ -2961,7 +4020,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>30</v>
       </c>
@@ -2972,7 +4031,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>31</v>
       </c>
@@ -2987,7 +4046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>32</v>
       </c>
@@ -2998,7 +4057,7 @@
       <c r="C27" s="6"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>33</v>
       </c>
@@ -3009,7 +4068,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="14" t="s">
         <v>22</v>
       </c>
@@ -3017,7 +4076,7 @@
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="46" t="s">
         <v>86</v>
       </c>
@@ -3028,7 +4087,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="15" t="s">
         <v>25</v>
       </c>
@@ -3051,7 +4110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7C60E3-5132-4EAF-A6AE-357FE13BC6C9}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -3059,36 +4118,36 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:6" s="25" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+    </row>
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -3108,7 +4167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -3130,7 +4189,7 @@
         <v>C.</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -3150,7 +4209,7 @@
         <v>C. Doe</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -3170,7 +4229,7 @@
         <v>John C.</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -3190,7 +4249,7 @@
         <v>Doe</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>64</v>
       </c>
@@ -3199,7 +4258,7 @@
         <v>John C. Doe</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -3210,7 +4269,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -3221,7 +4280,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -3233,7 +4292,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -3245,12 +4304,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -3262,7 +4321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3274,7 +4333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>64</v>
       </c>
@@ -3289,7 +4348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C83CC8-3284-4752-8E92-8CBBD1003835}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -3297,37 +4356,37 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:5" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -3335,7 +4394,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>68</v>
       </c>
@@ -3344,7 +4403,7 @@
         <v>3.1415929999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3353,7 +4412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -3362,20 +4421,20 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="51"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="56"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -3383,7 +4442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +4451,7 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>35</v>
       </c>
@@ -3400,13 +4459,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="7"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
@@ -3426,7 +4485,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B15AA95-D2AA-4AD6-8E83-DBFAD20B8498}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -3434,48 +4493,48 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="4" width="15.140625" customWidth="1"/>
+    <col min="3" max="4" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="52"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="41"/>
       <c r="D1" s="41"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="53"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" s="42" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="42" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="49" t="s">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="51"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="56"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B5" s="26"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
@@ -3483,13 +4542,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="17"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
         <v>40</v>
       </c>
@@ -3498,7 +4557,7 @@
         <v>Untitled Document.docx</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>42</v>
       </c>
@@ -3507,7 +4566,7 @@
         <v>docx</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="20" t="s">
         <v>41</v>
       </c>
@@ -3516,7 +4575,7 @@
         <v>Untitled Document</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="24" t="s">
         <v>56</v>
       </c>
@@ -3525,7 +4584,7 @@
         <v>C:\temp\</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>57</v>
       </c>
@@ -3544,122 +4603,122 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88115396-113A-4E92-ABEE-648E1977C738}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="165.5703125" style="30" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="30" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="30"/>
+    <col min="1" max="1" width="165.54296875" style="30" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="30" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7265625" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="36"/>
     </row>
-    <row r="2" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="35" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="37" x14ac:dyDescent="0.35">
       <c r="A3" s="38" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="35"/>
       <c r="D4" s="31"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="34" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="33"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="35"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="35"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="35"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="35"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="35"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="35"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="35"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="35"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="35"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="35"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="37" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="37" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="37" t="s">
         <v>75</v>
       </c>

</xml_diff>